<commit_message>
data baru trucking S1L untuk track area gudang
</commit_message>
<xml_diff>
--- a/Summary_Cabang_AB_2025 (Split).xlsx
+++ b/Summary_Cabang_AB_2025 (Split).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6EED2E-222C-4141-BFED-F63C358D0207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ED8B09-0BB0-4781-8DA6-46727EDA013B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="28" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMBON" sheetId="1" r:id="rId1"/>
@@ -25981,7 +25981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -55463,9 +55463,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:AL17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">

</xml_diff>